<commit_message>
emplyee and search age vaidation code added
</commit_message>
<xml_diff>
--- a/src/main/java/com/jala/qa/dataLayer/Book.xlsx
+++ b/src/main/java/com/jala/qa/dataLayer/Book.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19020" windowHeight="7740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:S25"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Fname</t>
   </si>
@@ -70,13 +73,34 @@
   </si>
   <si>
     <t>hyderabad</t>
+  </si>
+  <si>
+    <t>urname</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>rechard</t>
+  </si>
+  <si>
+    <t>lucky</t>
+  </si>
+  <si>
+    <t>lucky@gmail.com</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +115,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,11 +159,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -417,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,4 +569,95 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9999999999</v>
+      </c>
+      <c r="E2" s="4">
+        <v>38101</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>